<commit_message>
upload the image of towers and wizards
</commit_message>
<xml_diff>
--- a/docs/config/levels.xlsx
+++ b/docs/config/levels.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\yyy\software_engine\2025-group-5\Game\config\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\yyy\software_engine\2025-group-5\docs\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E0C6A2A-DB0D-4D3E-8BF9-8D887B8D8E08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ACC320B-B16F-4F7B-AF7D-FF129CF8FEC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{9F8622C9-03A3-4207-9844-CBC14631E7E3}"/>
+    <workbookView xWindow="19090" yWindow="-110" windowWidth="25820" windowHeight="16220" xr2:uid="{9F8622C9-03A3-4207-9844-CBC14631E7E3}"/>
   </bookViews>
   <sheets>
     <sheet name="level1" sheetId="1" r:id="rId1"/>
@@ -59,7 +59,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -69,12 +69,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="1"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -93,20 +87,17 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -423,49 +414,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25643E50-2057-49C8-B702-5569040FBAE3}">
-  <dimension ref="A3:AN25"/>
+  <dimension ref="A4:AN25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="V4" sqref="V4"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="AI14" sqref="AI14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="3.625" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="3" spans="1:40" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="T3" s="2"/>
-      <c r="U3" s="2"/>
-      <c r="V3" s="2"/>
-      <c r="W3" s="2"/>
-      <c r="X3" s="2"/>
-    </row>
     <row r="4" spans="1:40" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="N4" s="2"/>
-      <c r="O4" s="2"/>
-      <c r="P4" s="2"/>
-      <c r="Q4" s="2"/>
-      <c r="R4" s="2"/>
-      <c r="S4" s="2"/>
       <c r="T4" s="1"/>
       <c r="U4" s="1"/>
       <c r="V4" s="1"/>
       <c r="W4" s="1"/>
       <c r="X4" s="1"/>
-      <c r="Y4" s="2"/>
-      <c r="Z4" s="2"/>
-      <c r="AA4" s="4"/>
-      <c r="AB4" s="4"/>
-      <c r="AC4" s="4"/>
-      <c r="AD4" s="4"/>
-      <c r="AE4" s="4"/>
-      <c r="AF4" s="4"/>
-      <c r="AG4" s="4"/>
-      <c r="AH4" s="4"/>
-      <c r="AI4" s="4"/>
-      <c r="AJ4" s="4"/>
-      <c r="AK4" s="4"/>
-      <c r="AL4" s="4"/>
-      <c r="AM4" s="4"/>
-      <c r="AN4" s="4"/>
+      <c r="AA4" s="2"/>
+      <c r="AB4" s="2"/>
+      <c r="AC4" s="2"/>
+      <c r="AD4" s="2"/>
+      <c r="AE4" s="2"/>
+      <c r="AF4" s="2"/>
+      <c r="AG4" s="2"/>
+      <c r="AH4" s="2"/>
+      <c r="AI4" s="2"/>
+      <c r="AJ4" s="2"/>
+      <c r="AK4" s="2"/>
+      <c r="AL4" s="2"/>
+      <c r="AM4" s="2"/>
+      <c r="AN4" s="2"/>
     </row>
     <row r="5" spans="1:40" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="N5" s="1"/>
@@ -479,17 +455,11 @@
       <c r="Y5" s="1"/>
       <c r="Z5" s="1"/>
       <c r="AA5" s="1"/>
-      <c r="AB5" s="2"/>
-      <c r="AC5" s="2"/>
-      <c r="AD5" s="2"/>
       <c r="AE5" s="1"/>
       <c r="AF5" s="1"/>
-      <c r="AG5" s="2"/>
       <c r="AH5" s="1"/>
       <c r="AI5" s="1"/>
-      <c r="AJ5" s="2"/>
-      <c r="AK5" s="1"/>
-      <c r="AL5" s="2"/>
+      <c r="AK5" s="3"/>
       <c r="AM5" s="1"/>
       <c r="AN5" s="1"/>
     </row>
@@ -503,11 +473,7 @@
       <c r="AN6" s="1"/>
     </row>
     <row r="7" spans="1:40" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="N7" s="4"/>
-      <c r="T7" s="2"/>
-      <c r="U7" s="2"/>
-      <c r="V7" s="2"/>
-      <c r="W7" s="2"/>
+      <c r="N7" s="2"/>
       <c r="Z7" s="1"/>
       <c r="AA7" s="1"/>
       <c r="AE7" s="1"/>
@@ -519,18 +485,17 @@
       <c r="AN7" s="1"/>
     </row>
     <row r="8" spans="1:40" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="N8" s="4"/>
+      <c r="N8" s="2"/>
       <c r="T8" s="1"/>
       <c r="U8" s="1"/>
       <c r="V8" s="1"/>
       <c r="W8" s="1"/>
       <c r="Z8" s="1"/>
-      <c r="AA8" s="2"/>
       <c r="AL8" s="1"/>
       <c r="AN8" s="1"/>
     </row>
     <row r="9" spans="1:40" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="N9" s="4"/>
+      <c r="N9" s="2"/>
       <c r="T9" s="1"/>
       <c r="U9" s="1"/>
       <c r="V9" s="1"/>
@@ -539,7 +504,7 @@
       <c r="AN9" s="1"/>
     </row>
     <row r="10" spans="1:40" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="N10" s="4"/>
+      <c r="N10" s="2"/>
       <c r="P10" s="1"/>
       <c r="Q10" s="1"/>
       <c r="T10" s="1"/>
@@ -550,7 +515,7 @@
       <c r="AN10" s="1"/>
     </row>
     <row r="11" spans="1:40" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="N11" s="4"/>
+      <c r="N11" s="2"/>
       <c r="P11" s="1"/>
       <c r="Q11" s="1"/>
       <c r="Z11" s="1"/>
@@ -577,17 +542,9 @@
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
       <c r="H13" s="3"/>
-      <c r="I13" s="2"/>
-      <c r="J13" s="2"/>
-      <c r="K13" s="2"/>
       <c r="L13" s="1"/>
       <c r="M13" s="1"/>
-      <c r="N13" s="2"/>
       <c r="P13" s="1"/>
       <c r="Q13" s="1"/>
       <c r="Y13" s="1"/>
@@ -616,18 +573,8 @@
     </row>
     <row r="16" spans="1:40" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="1"/>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
       <c r="G16" s="1"/>
-      <c r="H16" s="2"/>
       <c r="I16" s="1"/>
-      <c r="J16" s="2"/>
-      <c r="K16" s="2"/>
-      <c r="L16" s="2"/>
-      <c r="M16" s="2"/>
       <c r="N16" s="1"/>
       <c r="P16" s="1"/>
       <c r="Q16" s="1"/>
@@ -639,9 +586,7 @@
     </row>
     <row r="17" spans="1:40" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="1"/>
-      <c r="D17" s="2"/>
       <c r="G17" s="1"/>
-      <c r="H17" s="2"/>
       <c r="P17" s="1"/>
       <c r="Q17" s="1"/>
       <c r="Z17" s="1"/>
@@ -650,9 +595,7 @@
     </row>
     <row r="18" spans="1:40" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="1"/>
-      <c r="D18" s="2"/>
       <c r="G18" s="1"/>
-      <c r="H18" s="2"/>
       <c r="J18" s="1"/>
       <c r="P18" s="1"/>
       <c r="Q18" s="1"/>
@@ -661,9 +604,6 @@
     </row>
     <row r="19" spans="1:40" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="1"/>
-      <c r="D19" s="2"/>
-      <c r="G19" s="2"/>
-      <c r="H19" s="2"/>
       <c r="P19" s="1"/>
       <c r="Q19" s="1"/>
       <c r="T19" s="1"/>
@@ -676,10 +616,6 @@
     <row r="20" spans="1:40" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
-      <c r="D20" s="2"/>
-      <c r="G20" s="2"/>
-      <c r="H20" s="2"/>
-      <c r="I20" s="2"/>
       <c r="T20" s="1"/>
       <c r="U20" s="1"/>
       <c r="V20" s="1"/>
@@ -690,10 +626,8 @@
     <row r="21" spans="1:40" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
-      <c r="D21" s="2"/>
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
-      <c r="I21" s="2"/>
       <c r="T21" s="1"/>
       <c r="U21" s="1"/>
       <c r="V21" s="1"/>
@@ -706,9 +640,7 @@
     </row>
     <row r="22" spans="1:40" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C22" s="1"/>
-      <c r="D22" s="2"/>
       <c r="G22" s="1"/>
-      <c r="I22" s="2"/>
       <c r="K22" s="1"/>
       <c r="L22" s="1"/>
       <c r="M22" s="1"/>

</xml_diff>

<commit_message>
configure level2, level3 and level4
</commit_message>
<xml_diff>
--- a/docs/config/levels.xlsx
+++ b/docs/config/levels.xlsx
@@ -8,12 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\yyy\software_engine\2025-group-5\docs\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ACC320B-B16F-4F7B-AF7D-FF129CF8FEC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{571E3501-F3F2-48F1-BFEE-68ED288654D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19090" yWindow="-110" windowWidth="25820" windowHeight="16220" xr2:uid="{9F8622C9-03A3-4207-9844-CBC14631E7E3}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="3" xr2:uid="{9F8622C9-03A3-4207-9844-CBC14631E7E3}"/>
   </bookViews>
   <sheets>
     <sheet name="level1" sheetId="1" r:id="rId1"/>
+    <sheet name="level2" sheetId="2" r:id="rId2"/>
+    <sheet name="level3" sheetId="3" r:id="rId3"/>
+    <sheet name="level4" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,9 +36,13 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -58,6 +65,13 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -73,12 +87,48 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="5">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -87,7 +137,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -97,7 +147,31 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -416,13 +490,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25643E50-2057-49C8-B702-5569040FBAE3}">
   <dimension ref="A4:AN25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="AI14" sqref="AI14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="AM14" sqref="AM14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="3.625" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="3.58203125" defaultRowHeight="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="4" spans="1:40" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:40" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="T4" s="1"/>
       <c r="U4" s="1"/>
       <c r="V4" s="1"/>
@@ -443,7 +517,7 @@
       <c r="AM4" s="2"/>
       <c r="AN4" s="2"/>
     </row>
-    <row r="5" spans="1:40" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:40" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="N5" s="1"/>
       <c r="O5" s="1"/>
       <c r="P5" s="1"/>
@@ -459,11 +533,10 @@
       <c r="AF5" s="1"/>
       <c r="AH5" s="1"/>
       <c r="AI5" s="1"/>
-      <c r="AK5" s="3"/>
       <c r="AM5" s="1"/>
       <c r="AN5" s="1"/>
     </row>
-    <row r="6" spans="1:40" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:40" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="N6" s="1"/>
       <c r="Z6" s="1"/>
       <c r="AA6" s="1"/>
@@ -472,7 +545,7 @@
       <c r="AH6" s="1"/>
       <c r="AN6" s="1"/>
     </row>
-    <row r="7" spans="1:40" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:40" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="N7" s="2"/>
       <c r="Z7" s="1"/>
       <c r="AA7" s="1"/>
@@ -484,7 +557,7 @@
       <c r="AK7" s="1"/>
       <c r="AN7" s="1"/>
     </row>
-    <row r="8" spans="1:40" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:40" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="N8" s="2"/>
       <c r="T8" s="1"/>
       <c r="U8" s="1"/>
@@ -494,7 +567,7 @@
       <c r="AL8" s="1"/>
       <c r="AN8" s="1"/>
     </row>
-    <row r="9" spans="1:40" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:40" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="N9" s="2"/>
       <c r="T9" s="1"/>
       <c r="U9" s="1"/>
@@ -503,7 +576,7 @@
       <c r="Z9" s="1"/>
       <c r="AN9" s="1"/>
     </row>
-    <row r="10" spans="1:40" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:40" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="N10" s="2"/>
       <c r="P10" s="1"/>
       <c r="Q10" s="1"/>
@@ -514,14 +587,14 @@
       <c r="Z10" s="1"/>
       <c r="AN10" s="1"/>
     </row>
-    <row r="11" spans="1:40" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:40" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="N11" s="2"/>
       <c r="P11" s="1"/>
       <c r="Q11" s="1"/>
       <c r="Z11" s="1"/>
       <c r="AN11" s="1"/>
     </row>
-    <row r="12" spans="1:40" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:40" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
@@ -538,11 +611,10 @@
       <c r="AA12" s="1"/>
       <c r="AN12" s="1"/>
     </row>
-    <row r="13" spans="1:40" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:40" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
-      <c r="H13" s="3"/>
       <c r="L13" s="1"/>
       <c r="M13" s="1"/>
       <c r="P13" s="1"/>
@@ -553,7 +625,7 @@
       <c r="AH13" s="1"/>
       <c r="AN13" s="1"/>
     </row>
-    <row r="14" spans="1:40" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:40" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="P14" s="1"/>
       <c r="Q14" s="1"/>
       <c r="S14" s="1"/>
@@ -562,7 +634,7 @@
       <c r="AH14" s="1"/>
       <c r="AN14" s="1"/>
     </row>
-    <row r="15" spans="1:40" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:40" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="P15" s="1"/>
       <c r="Q15" s="1"/>
       <c r="S15" s="1"/>
@@ -571,7 +643,7 @@
       <c r="AH15" s="1"/>
       <c r="AN15" s="1"/>
     </row>
-    <row r="16" spans="1:40" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:40" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1"/>
       <c r="G16" s="1"/>
       <c r="I16" s="1"/>
@@ -584,7 +656,7 @@
       <c r="AH16" s="1"/>
       <c r="AN16" s="1"/>
     </row>
-    <row r="17" spans="1:40" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:40" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1"/>
       <c r="G17" s="1"/>
       <c r="P17" s="1"/>
@@ -593,7 +665,7 @@
       <c r="AA17" s="1"/>
       <c r="AN17" s="1"/>
     </row>
-    <row r="18" spans="1:40" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:40" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1"/>
       <c r="G18" s="1"/>
       <c r="J18" s="1"/>
@@ -602,7 +674,7 @@
       <c r="Z18" s="1"/>
       <c r="AN18" s="1"/>
     </row>
-    <row r="19" spans="1:40" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:40" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1"/>
       <c r="P19" s="1"/>
       <c r="Q19" s="1"/>
@@ -613,7 +685,7 @@
       <c r="Z19" s="1"/>
       <c r="AN19" s="1"/>
     </row>
-    <row r="20" spans="1:40" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:40" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="T20" s="1"/>
@@ -623,7 +695,7 @@
       <c r="Z20" s="1"/>
       <c r="AN20" s="1"/>
     </row>
-    <row r="21" spans="1:40" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:40" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
       <c r="G21" s="1"/>
@@ -638,7 +710,7 @@
       <c r="AC21" s="1"/>
       <c r="AN21" s="1"/>
     </row>
-    <row r="22" spans="1:40" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:40" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C22" s="1"/>
       <c r="G22" s="1"/>
       <c r="K22" s="1"/>
@@ -654,7 +726,7 @@
       <c r="AM22" s="1"/>
       <c r="AN22" s="1"/>
     </row>
-    <row r="23" spans="1:40" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:40" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
       <c r="G23" s="1"/>
@@ -668,7 +740,7 @@
       <c r="AJ23" s="1"/>
       <c r="AN23" s="1"/>
     </row>
-    <row r="24" spans="1:40" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:40" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D24" s="1"/>
       <c r="G24" s="1"/>
       <c r="H24" s="1"/>
@@ -685,7 +757,7 @@
       <c r="AJ24" s="1"/>
       <c r="AN24" s="1"/>
     </row>
-    <row r="25" spans="1:40" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:40" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D25" s="1"/>
       <c r="G25" s="1"/>
       <c r="O25" s="1"/>
@@ -714,4 +786,1166 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D787DCD7-EEC2-4EBB-96A8-62870AA97245}">
+  <dimension ref="A1:AN25"/>
+  <sheetViews>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="AR7" sqref="AR7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="3.58203125" defaultRowHeight="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:40" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="R1" s="1"/>
+      <c r="S1" s="1"/>
+      <c r="T1" s="1"/>
+      <c r="U1" s="1"/>
+      <c r="V1" s="1"/>
+      <c r="AN1" s="1"/>
+    </row>
+    <row r="2" spans="1:40" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="G2" s="1"/>
+      <c r="J2" s="1"/>
+      <c r="M2" s="1"/>
+      <c r="R2" s="1"/>
+      <c r="S2" s="1"/>
+      <c r="T2" s="1"/>
+      <c r="U2" s="1"/>
+      <c r="V2" s="1"/>
+      <c r="AN2" s="1"/>
+    </row>
+    <row r="3" spans="1:40" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="M3" s="1"/>
+      <c r="R3" s="1"/>
+      <c r="S3" s="1"/>
+      <c r="T3" s="1"/>
+      <c r="U3" s="1"/>
+      <c r="V3" s="1"/>
+      <c r="AN3" s="1"/>
+    </row>
+    <row r="4" spans="1:40" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="M4" s="1"/>
+      <c r="R4" s="1"/>
+      <c r="S4" s="1"/>
+      <c r="T4" s="1"/>
+      <c r="U4" s="1"/>
+      <c r="V4" s="1"/>
+      <c r="AN4" s="1"/>
+    </row>
+    <row r="5" spans="1:40" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="M5" s="1"/>
+      <c r="R5" s="1"/>
+      <c r="S5" s="1"/>
+      <c r="T5" s="1"/>
+      <c r="U5" s="1"/>
+      <c r="V5" s="1"/>
+      <c r="AN5" s="1"/>
+    </row>
+    <row r="6" spans="1:40" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="M6" s="1"/>
+      <c r="R6" s="1"/>
+      <c r="S6" s="1"/>
+      <c r="T6" s="1"/>
+      <c r="U6" s="1"/>
+      <c r="V6" s="1"/>
+      <c r="AN6" s="1"/>
+    </row>
+    <row r="7" spans="1:40" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="M7" s="1"/>
+      <c r="R7" s="1"/>
+      <c r="S7" s="1"/>
+      <c r="T7" s="1"/>
+      <c r="U7" s="1"/>
+      <c r="V7" s="1"/>
+      <c r="AN7" s="1"/>
+    </row>
+    <row r="8" spans="1:40" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="M8" s="1"/>
+      <c r="R8" s="1"/>
+      <c r="S8" s="1"/>
+      <c r="T8" s="1"/>
+      <c r="U8" s="1"/>
+      <c r="V8" s="1"/>
+      <c r="AE8" s="1"/>
+      <c r="AF8" s="1"/>
+      <c r="AG8" s="1"/>
+      <c r="AN8" s="1"/>
+    </row>
+    <row r="9" spans="1:40" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="M9" s="1"/>
+      <c r="R9" s="1"/>
+      <c r="S9" s="1"/>
+      <c r="T9" s="1"/>
+      <c r="U9" s="1"/>
+      <c r="V9" s="1"/>
+      <c r="AA9" s="1"/>
+      <c r="AB9" s="1"/>
+      <c r="AC9" s="1"/>
+      <c r="AD9" s="1"/>
+      <c r="AE9" s="1"/>
+      <c r="AF9" s="1"/>
+      <c r="AG9" s="1"/>
+      <c r="AN9" s="1"/>
+    </row>
+    <row r="10" spans="1:40" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+      <c r="M10" s="1"/>
+      <c r="R10" s="1"/>
+      <c r="S10" s="1"/>
+      <c r="T10" s="1"/>
+      <c r="U10" s="1"/>
+      <c r="V10" s="1"/>
+      <c r="AA10" s="1"/>
+      <c r="AB10" s="1"/>
+      <c r="AE10" s="1"/>
+      <c r="AF10" s="1"/>
+      <c r="AG10" s="1"/>
+      <c r="AI10" s="1"/>
+      <c r="AJ10" s="1"/>
+      <c r="AN10" s="1"/>
+    </row>
+    <row r="11" spans="1:40" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
+      <c r="K11" s="1"/>
+      <c r="L11" s="1"/>
+      <c r="M11" s="1"/>
+      <c r="R11" s="1"/>
+      <c r="S11" s="1"/>
+      <c r="T11" s="1"/>
+      <c r="U11" s="1"/>
+      <c r="V11" s="1"/>
+      <c r="AB11" s="1"/>
+      <c r="AC11" s="1"/>
+      <c r="AE11" s="1"/>
+      <c r="AF11" s="1"/>
+      <c r="AG11" s="1"/>
+      <c r="AI11" s="1"/>
+      <c r="AJ11" s="1"/>
+      <c r="AK11" s="1"/>
+      <c r="AL11" s="1"/>
+      <c r="AM11" s="1"/>
+      <c r="AN11" s="1"/>
+    </row>
+    <row r="12" spans="1:40" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+      <c r="K12" s="1"/>
+      <c r="L12" s="1"/>
+      <c r="M12" s="1"/>
+      <c r="R12" s="1"/>
+      <c r="S12" s="1"/>
+      <c r="T12" s="1"/>
+      <c r="U12" s="1"/>
+      <c r="V12" s="1"/>
+      <c r="W12" s="1"/>
+      <c r="X12" s="1"/>
+      <c r="Y12" s="1"/>
+      <c r="Z12" s="1"/>
+      <c r="AA12" s="1"/>
+      <c r="AB12" s="1"/>
+      <c r="AC12" s="1"/>
+      <c r="AE12" s="1"/>
+      <c r="AH12" s="1"/>
+      <c r="AI12" s="1"/>
+      <c r="AJ12" s="1"/>
+      <c r="AK12" s="1"/>
+      <c r="AN12" s="1"/>
+    </row>
+    <row r="13" spans="1:40" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+      <c r="K13" s="1"/>
+      <c r="L13" s="1"/>
+      <c r="M13" s="1"/>
+      <c r="N13" s="1"/>
+      <c r="O13" s="1"/>
+      <c r="R13" s="1"/>
+      <c r="Y13" s="1"/>
+      <c r="AH13" s="1"/>
+      <c r="AN13" s="1"/>
+    </row>
+    <row r="14" spans="1:40" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+    </row>
+    <row r="15" spans="1:40" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="AG15" s="1"/>
+    </row>
+    <row r="16" spans="1:40" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="I16" s="1"/>
+      <c r="J16" s="1"/>
+      <c r="K16" s="1"/>
+      <c r="L16" s="1"/>
+      <c r="M16" s="1"/>
+      <c r="N16" s="1"/>
+      <c r="O16" s="1"/>
+      <c r="AG16" s="1"/>
+      <c r="AK16" s="1"/>
+      <c r="AM16" s="1"/>
+      <c r="AN16" s="1"/>
+    </row>
+    <row r="17" spans="1:40" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="1"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="I17" s="1"/>
+      <c r="J17" s="1"/>
+      <c r="K17" s="1"/>
+      <c r="L17" s="1"/>
+      <c r="M17" s="1"/>
+      <c r="R17" s="1"/>
+      <c r="S17" s="1"/>
+      <c r="V17" s="1"/>
+      <c r="W17" s="1"/>
+      <c r="X17" s="1"/>
+      <c r="Y17" s="1"/>
+      <c r="Z17" s="1"/>
+      <c r="AA17" s="1"/>
+      <c r="AB17" s="1"/>
+      <c r="AC17" s="1"/>
+      <c r="AD17" s="1"/>
+      <c r="AE17" s="1"/>
+      <c r="AF17" s="1"/>
+      <c r="AL17" s="1"/>
+      <c r="AM17" s="1"/>
+      <c r="AN17" s="1"/>
+    </row>
+    <row r="18" spans="1:40" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="1"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="I18" s="1"/>
+      <c r="J18" s="1"/>
+      <c r="K18" s="1"/>
+      <c r="L18" s="1"/>
+      <c r="M18" s="1"/>
+      <c r="N18" s="1"/>
+      <c r="O18" s="1"/>
+      <c r="P18" s="1"/>
+      <c r="R18" s="1"/>
+      <c r="S18" s="1"/>
+      <c r="T18" s="1"/>
+      <c r="U18" s="1"/>
+      <c r="V18" s="1"/>
+      <c r="W18" s="1"/>
+      <c r="X18" s="1"/>
+      <c r="Y18" s="1"/>
+      <c r="Z18" s="1"/>
+      <c r="AA18" s="1"/>
+      <c r="AB18" s="1"/>
+      <c r="AC18" s="1"/>
+      <c r="AD18" s="1"/>
+      <c r="AE18" s="1"/>
+      <c r="AF18" s="1"/>
+      <c r="AL18" s="1"/>
+      <c r="AM18" s="1"/>
+      <c r="AN18" s="1"/>
+    </row>
+    <row r="19" spans="1:40" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="1"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="M19" s="1"/>
+      <c r="N19" s="1"/>
+      <c r="O19" s="1"/>
+      <c r="P19" s="1"/>
+      <c r="R19" s="1"/>
+      <c r="S19" s="1"/>
+      <c r="T19" s="1"/>
+      <c r="U19" s="1"/>
+      <c r="V19" s="1"/>
+      <c r="W19" s="1"/>
+      <c r="X19" s="1"/>
+      <c r="Y19" s="1"/>
+      <c r="Z19" s="1"/>
+      <c r="AA19" s="1"/>
+      <c r="AB19" s="1"/>
+      <c r="AC19" s="1"/>
+      <c r="AD19" s="1"/>
+      <c r="AE19" s="1"/>
+      <c r="AF19" s="1"/>
+      <c r="AL19" s="1"/>
+      <c r="AM19" s="1"/>
+      <c r="AN19" s="1"/>
+    </row>
+    <row r="20" spans="1:40" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="1"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="M20" s="1"/>
+      <c r="N20" s="1"/>
+      <c r="O20" s="1"/>
+      <c r="P20" s="1"/>
+      <c r="R20" s="1"/>
+      <c r="S20" s="1"/>
+      <c r="V20" s="1"/>
+      <c r="W20" s="1"/>
+      <c r="X20" s="1"/>
+      <c r="Y20" s="1"/>
+      <c r="Z20" s="1"/>
+      <c r="AA20" s="1"/>
+      <c r="AB20" s="1"/>
+      <c r="AC20" s="1"/>
+      <c r="AD20" s="1"/>
+      <c r="AE20" s="1"/>
+      <c r="AF20" s="1"/>
+      <c r="AL20" s="1"/>
+      <c r="AM20" s="1"/>
+      <c r="AN20" s="1"/>
+    </row>
+    <row r="21" spans="1:40" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="1"/>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="M21" s="1"/>
+      <c r="N21" s="1"/>
+      <c r="O21" s="1"/>
+      <c r="P21" s="1"/>
+      <c r="Q21" s="1"/>
+      <c r="R21" s="1"/>
+      <c r="S21" s="1"/>
+      <c r="AL21" s="1"/>
+      <c r="AM21" s="1"/>
+      <c r="AN21" s="1"/>
+    </row>
+    <row r="22" spans="1:40" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="1"/>
+      <c r="M22" s="1"/>
+      <c r="N22" s="1"/>
+      <c r="O22" s="1"/>
+      <c r="P22" s="1"/>
+      <c r="Q22" s="1"/>
+      <c r="R22" s="1"/>
+      <c r="S22" s="1"/>
+      <c r="V22" s="1"/>
+      <c r="W22" s="1"/>
+      <c r="X22" s="1"/>
+      <c r="Y22" s="1"/>
+      <c r="Z22" s="1"/>
+      <c r="AA22" s="1"/>
+      <c r="AB22" s="1"/>
+      <c r="AC22" s="1"/>
+      <c r="AD22" s="1"/>
+      <c r="AE22" s="1"/>
+      <c r="AF22" s="1"/>
+      <c r="AL22" s="1"/>
+      <c r="AM22" s="1"/>
+      <c r="AN22" s="1"/>
+    </row>
+    <row r="23" spans="1:40" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="M23" s="1"/>
+      <c r="N23" s="1"/>
+      <c r="O23" s="1"/>
+      <c r="P23" s="1"/>
+      <c r="Q23" s="1"/>
+      <c r="R23" s="1"/>
+      <c r="S23" s="1"/>
+      <c r="V23" s="1"/>
+      <c r="W23" s="1"/>
+      <c r="X23" s="1"/>
+      <c r="Y23" s="1"/>
+      <c r="Z23" s="1"/>
+      <c r="AA23" s="1"/>
+      <c r="AB23" s="1"/>
+      <c r="AC23" s="1"/>
+      <c r="AD23" s="1"/>
+      <c r="AE23" s="1"/>
+      <c r="AF23" s="1"/>
+      <c r="AL23" s="1"/>
+      <c r="AM23" s="1"/>
+      <c r="AN23" s="1"/>
+    </row>
+    <row r="24" spans="1:40" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="1"/>
+      <c r="M24" s="1"/>
+      <c r="N24" s="1"/>
+      <c r="O24" s="1"/>
+      <c r="P24" s="1"/>
+      <c r="Q24" s="1"/>
+      <c r="R24" s="1"/>
+      <c r="S24" s="1"/>
+      <c r="T24" s="1"/>
+      <c r="U24" s="1"/>
+      <c r="X24" s="1"/>
+      <c r="Y24" s="1"/>
+      <c r="AA24" s="1"/>
+      <c r="AB24" s="1"/>
+      <c r="AM24" s="1"/>
+      <c r="AN24" s="1"/>
+    </row>
+    <row r="25" spans="1:40" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="1"/>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
+      <c r="H25" s="1"/>
+      <c r="I25" s="1"/>
+      <c r="J25" s="1"/>
+      <c r="K25" s="1"/>
+      <c r="L25" s="1"/>
+      <c r="M25" s="1"/>
+      <c r="N25" s="1"/>
+      <c r="O25" s="1"/>
+      <c r="P25" s="1"/>
+      <c r="T25" s="1"/>
+      <c r="U25" s="1"/>
+      <c r="X25" s="1"/>
+      <c r="Y25" s="1"/>
+      <c r="AC25" s="1"/>
+      <c r="AD25" s="1"/>
+      <c r="AH25" s="1"/>
+      <c r="AK25" s="1"/>
+      <c r="AM25" s="1"/>
+      <c r="AN25" s="1"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06D6D923-E7BC-4682-801E-F4EAC126B44A}">
+  <dimension ref="A1:AO27"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J18" sqref="J18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="3.58203125" defaultRowHeight="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:41" ht="20.149999999999999" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="F1" s="3"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="3"/>
+      <c r="Z1" s="3"/>
+      <c r="AA1" s="4"/>
+      <c r="AB1" s="4"/>
+      <c r="AC1" s="4"/>
+      <c r="AD1" s="4"/>
+      <c r="AE1" s="4"/>
+      <c r="AF1" s="4"/>
+      <c r="AG1" s="4"/>
+      <c r="AH1" s="4"/>
+      <c r="AI1" s="3"/>
+    </row>
+    <row r="2" spans="1:41" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F2" s="1"/>
+      <c r="H2" s="1"/>
+      <c r="Z2" s="1"/>
+      <c r="AI2" s="1"/>
+    </row>
+    <row r="3" spans="1:41" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1"/>
+      <c r="Y3" s="1"/>
+      <c r="AI3" s="1"/>
+    </row>
+    <row r="4" spans="1:41" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="N4" s="1"/>
+      <c r="O4" s="1"/>
+      <c r="P4" s="1"/>
+      <c r="Q4" s="1"/>
+      <c r="R4" s="1"/>
+      <c r="S4" s="1"/>
+      <c r="T4" s="1"/>
+      <c r="U4" s="1"/>
+      <c r="V4" s="1"/>
+      <c r="W4" s="1"/>
+      <c r="X4" s="1"/>
+      <c r="Y4" s="1"/>
+      <c r="AA4" s="5"/>
+      <c r="AB4" s="5"/>
+      <c r="AC4" s="5"/>
+      <c r="AD4" s="5"/>
+      <c r="AE4" s="5"/>
+      <c r="AF4" s="5"/>
+      <c r="AG4" s="5"/>
+      <c r="AH4" s="6"/>
+      <c r="AI4" s="6"/>
+      <c r="AJ4" s="6"/>
+      <c r="AK4" s="6"/>
+      <c r="AL4" s="6"/>
+      <c r="AM4" s="6"/>
+      <c r="AN4" s="7"/>
+    </row>
+    <row r="5" spans="1:41" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+    </row>
+    <row r="6" spans="1:41" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D6" s="1"/>
+      <c r="P6" s="1"/>
+      <c r="Q6" s="1"/>
+      <c r="R6" s="1"/>
+      <c r="S6" s="1"/>
+      <c r="T6" s="1"/>
+      <c r="U6" s="1"/>
+      <c r="V6" s="1"/>
+      <c r="W6" s="1"/>
+      <c r="X6" s="1"/>
+      <c r="Y6" s="1"/>
+      <c r="AH6" s="1"/>
+      <c r="AI6" s="1"/>
+      <c r="AJ6" s="1"/>
+      <c r="AK6" s="1"/>
+      <c r="AL6" s="1"/>
+      <c r="AM6" s="1"/>
+      <c r="AN6" s="8"/>
+    </row>
+    <row r="7" spans="1:41" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D7" s="1"/>
+      <c r="N7" s="6"/>
+      <c r="O7" s="1"/>
+      <c r="P7" s="1"/>
+      <c r="X7" s="1"/>
+      <c r="Y7" s="1"/>
+      <c r="AC7" s="1"/>
+      <c r="AD7" s="1"/>
+      <c r="AE7" s="1"/>
+      <c r="AF7" s="1"/>
+      <c r="AI7" s="1"/>
+      <c r="AJ7" s="1"/>
+    </row>
+    <row r="8" spans="1:41" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="9"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="N8" s="6"/>
+      <c r="X8" s="1"/>
+      <c r="AC8" s="1"/>
+      <c r="AF8" s="1"/>
+      <c r="AK8" s="1"/>
+    </row>
+    <row r="9" spans="1:41" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="10"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="1"/>
+      <c r="L9" s="1"/>
+      <c r="N9" s="6"/>
+      <c r="O9" s="1"/>
+      <c r="X9" s="1"/>
+      <c r="AC9" s="1"/>
+      <c r="AD9" s="1"/>
+      <c r="AE9" s="1"/>
+      <c r="AF9" s="1"/>
+      <c r="AH9" s="1"/>
+      <c r="AI9" s="1"/>
+      <c r="AJ9" s="1"/>
+      <c r="AK9" s="1"/>
+    </row>
+    <row r="10" spans="1:41" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="9"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="H10" s="1"/>
+      <c r="L10" s="1"/>
+      <c r="N10" s="5"/>
+      <c r="O10" s="1"/>
+      <c r="X10" s="1"/>
+      <c r="AH10" s="1"/>
+    </row>
+    <row r="11" spans="1:41" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
+      <c r="K11" s="1"/>
+      <c r="N11" s="5"/>
+      <c r="O11" s="1"/>
+      <c r="Y11" s="1"/>
+      <c r="Z11" s="1"/>
+      <c r="AH11" s="1"/>
+    </row>
+    <row r="12" spans="1:41" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="1"/>
+      <c r="K12" s="1"/>
+      <c r="O12" s="1"/>
+      <c r="AA12" s="1"/>
+      <c r="AC12" s="1"/>
+      <c r="AD12" s="1"/>
+      <c r="AF12" s="1"/>
+      <c r="AG12" s="1"/>
+      <c r="AH12" s="1"/>
+    </row>
+    <row r="13" spans="1:41" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="J13" s="1"/>
+      <c r="K13" s="1"/>
+      <c r="L13" s="1"/>
+      <c r="M13" s="1"/>
+      <c r="O13" s="1"/>
+      <c r="AA13" s="1"/>
+      <c r="AC13" s="1"/>
+      <c r="AE13" s="1"/>
+      <c r="AF13" s="1"/>
+    </row>
+    <row r="14" spans="1:41" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="J14" s="1"/>
+      <c r="M14" s="1"/>
+      <c r="O14" s="1"/>
+      <c r="AA14" s="1"/>
+      <c r="AC14" s="1"/>
+    </row>
+    <row r="15" spans="1:41" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="1"/>
+      <c r="M15" s="1"/>
+      <c r="O15" s="1"/>
+      <c r="AA15" s="1"/>
+      <c r="AC15" s="1"/>
+      <c r="AN15" s="8"/>
+    </row>
+    <row r="16" spans="1:41" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="M16" s="1"/>
+      <c r="O16" s="1"/>
+      <c r="AA16" s="1"/>
+      <c r="AC16" s="1"/>
+      <c r="AM16" s="1"/>
+      <c r="AN16" s="5"/>
+      <c r="AO16" s="5"/>
+    </row>
+    <row r="17" spans="1:41" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="M17" s="1"/>
+      <c r="O17" s="1"/>
+      <c r="T17" s="1"/>
+      <c r="U17" s="1"/>
+      <c r="V17" s="1"/>
+      <c r="W17" s="1"/>
+      <c r="X17" s="1"/>
+      <c r="Y17" s="1"/>
+      <c r="Z17" s="1"/>
+      <c r="AA17" s="1"/>
+      <c r="AC17" s="1"/>
+      <c r="AL17" s="1"/>
+      <c r="AN17" s="5"/>
+      <c r="AO17" s="5"/>
+    </row>
+    <row r="18" spans="1:41" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="9"/>
+      <c r="B18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="M18" s="1"/>
+      <c r="O18" s="1"/>
+      <c r="S18" s="1"/>
+      <c r="Z18" s="1"/>
+      <c r="AA18" s="1"/>
+      <c r="AC18" s="1"/>
+      <c r="AK18" s="1"/>
+      <c r="AN18" s="5"/>
+      <c r="AO18" s="5"/>
+    </row>
+    <row r="19" spans="1:41" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="M19" s="1"/>
+      <c r="P19" s="1"/>
+      <c r="Q19" s="1"/>
+      <c r="R19" s="1"/>
+      <c r="AC19" s="1"/>
+      <c r="AD19" s="1"/>
+      <c r="AJ19" s="1"/>
+      <c r="AN19" s="5"/>
+      <c r="AO19" s="5"/>
+    </row>
+    <row r="20" spans="1:41" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="M20" s="1"/>
+      <c r="AD20" s="1"/>
+      <c r="AJ20" s="1"/>
+      <c r="AN20" s="5"/>
+      <c r="AO20" s="5"/>
+    </row>
+    <row r="21" spans="1:41" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+      <c r="M21" s="1"/>
+      <c r="N21" s="1"/>
+      <c r="O21" s="1"/>
+      <c r="U21" s="1"/>
+      <c r="V21" s="1"/>
+      <c r="W21" s="1"/>
+      <c r="AD21" s="1"/>
+      <c r="AJ21" s="1"/>
+      <c r="AN21" s="5"/>
+      <c r="AO21" s="5"/>
+    </row>
+    <row r="22" spans="1:41" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1"/>
+      <c r="I22" s="1"/>
+      <c r="J22" s="1"/>
+      <c r="K22" s="1"/>
+      <c r="L22" s="1"/>
+      <c r="M22" s="1"/>
+      <c r="N22" s="1"/>
+      <c r="O22" s="1"/>
+      <c r="U22" s="1"/>
+      <c r="W22" s="1"/>
+      <c r="AD22" s="1"/>
+      <c r="AE22" s="1"/>
+      <c r="AF22" s="1"/>
+      <c r="AG22" s="1"/>
+      <c r="AH22" s="1"/>
+      <c r="AI22" s="1"/>
+      <c r="AJ22" s="1"/>
+      <c r="AN22" s="5"/>
+      <c r="AO22" s="5"/>
+    </row>
+    <row r="23" spans="1:41" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="U23" s="1"/>
+      <c r="V23" s="1"/>
+      <c r="W23" s="1"/>
+      <c r="AN23" s="5"/>
+      <c r="AO23" s="5"/>
+    </row>
+    <row r="24" spans="1:41" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H24" s="1"/>
+      <c r="I24" s="1"/>
+      <c r="J24" s="1"/>
+      <c r="K24" s="1"/>
+      <c r="L24" s="1"/>
+      <c r="M24" s="1"/>
+      <c r="N24" s="1"/>
+      <c r="O24" s="1"/>
+      <c r="AE24" s="1"/>
+      <c r="AF24" s="1"/>
+      <c r="AG24" s="1"/>
+      <c r="AH24" s="1"/>
+      <c r="AI24" s="1"/>
+      <c r="AN24" s="5"/>
+      <c r="AO24" s="5"/>
+    </row>
+    <row r="25" spans="1:41" ht="20.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="I25" s="11"/>
+      <c r="P25" s="11"/>
+      <c r="Z25" s="11"/>
+      <c r="AA25" s="11"/>
+      <c r="AB25" s="11"/>
+      <c r="AC25" s="11"/>
+      <c r="AD25" s="11"/>
+      <c r="AE25" s="11"/>
+      <c r="AG25" s="11"/>
+      <c r="AH25" s="5"/>
+      <c r="AI25" s="5"/>
+      <c r="AJ25" s="5"/>
+      <c r="AK25" s="5"/>
+      <c r="AL25" s="5"/>
+      <c r="AM25" s="5"/>
+      <c r="AN25" s="5"/>
+      <c r="AO25" s="5"/>
+    </row>
+    <row r="26" spans="1:41" ht="20.149999999999999" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="AH26" s="5"/>
+      <c r="AI26" s="5"/>
+      <c r="AJ26" s="5"/>
+      <c r="AK26" s="5"/>
+      <c r="AL26" s="5"/>
+      <c r="AM26" s="5"/>
+      <c r="AN26" s="5"/>
+    </row>
+    <row r="27" spans="1:41" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AH27" s="5"/>
+      <c r="AI27" s="5"/>
+      <c r="AJ27" s="5"/>
+      <c r="AK27" s="5"/>
+      <c r="AL27" s="5"/>
+      <c r="AM27" s="5"/>
+      <c r="AN27" s="5"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B873F3A3-FC30-4AC8-9328-E2AAE444BD5F}">
+  <dimension ref="A2:AN21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="S30" sqref="S30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="3.58203125" defaultRowHeight="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="2" spans="1:40" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="K2" s="1"/>
+      <c r="L2" s="1"/>
+      <c r="M2" s="1"/>
+      <c r="N2" s="1"/>
+      <c r="O2" s="1"/>
+      <c r="P2" s="1"/>
+      <c r="Q2" s="1"/>
+      <c r="R2" s="1"/>
+      <c r="S2" s="1"/>
+      <c r="T2" s="1"/>
+    </row>
+    <row r="3" spans="1:40" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="T3" s="1"/>
+    </row>
+    <row r="4" spans="1:40" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I4" s="1"/>
+      <c r="T4" s="1"/>
+      <c r="Z4" s="1"/>
+      <c r="AA4" s="6"/>
+      <c r="AB4" s="6"/>
+      <c r="AC4" s="6"/>
+      <c r="AD4" s="6"/>
+      <c r="AE4" s="6"/>
+      <c r="AF4" s="6"/>
+      <c r="AG4" s="6"/>
+      <c r="AH4" s="6"/>
+      <c r="AI4" s="6"/>
+      <c r="AJ4" s="6"/>
+      <c r="AK4" s="6"/>
+      <c r="AL4" s="6"/>
+      <c r="AM4" s="6"/>
+      <c r="AN4" s="7"/>
+    </row>
+    <row r="5" spans="1:40" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I5" s="1"/>
+      <c r="T5" s="1"/>
+      <c r="U5" s="1"/>
+      <c r="V5" s="1"/>
+      <c r="W5" s="1"/>
+      <c r="X5" s="1"/>
+      <c r="Y5" s="1"/>
+      <c r="Z5" s="1"/>
+    </row>
+    <row r="6" spans="1:40" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I6" s="1"/>
+    </row>
+    <row r="7" spans="1:40" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I7" s="1"/>
+      <c r="T7" s="1"/>
+      <c r="U7" s="1"/>
+      <c r="V7" s="1"/>
+      <c r="W7" s="1"/>
+      <c r="X7" s="1"/>
+      <c r="Y7" s="1"/>
+      <c r="Z7" s="1"/>
+      <c r="AK7" s="1"/>
+    </row>
+    <row r="8" spans="1:40" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="9"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+      <c r="N8" s="5"/>
+      <c r="T8" s="1"/>
+      <c r="Z8" s="1"/>
+    </row>
+    <row r="9" spans="1:40" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="J9" s="1"/>
+      <c r="N9" s="5"/>
+      <c r="O9" s="1"/>
+      <c r="T9" s="1"/>
+      <c r="Z9" s="1"/>
+      <c r="AE9" s="1"/>
+      <c r="AF9" s="1"/>
+      <c r="AG9" s="1"/>
+      <c r="AH9" s="1"/>
+      <c r="AI9" s="1"/>
+      <c r="AK9" s="1"/>
+      <c r="AL9" s="1"/>
+      <c r="AM9" s="1"/>
+      <c r="AN9" s="8"/>
+    </row>
+    <row r="10" spans="1:40" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="N10" s="5"/>
+      <c r="T10" s="1"/>
+      <c r="U10" s="1"/>
+      <c r="V10" s="1"/>
+      <c r="W10" s="1"/>
+      <c r="X10" s="1"/>
+      <c r="Z10" s="1"/>
+      <c r="AE10" s="1"/>
+      <c r="AI10" s="1"/>
+      <c r="AK10" s="1"/>
+    </row>
+    <row r="11" spans="1:40" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="N11" s="5"/>
+      <c r="X11" s="1"/>
+      <c r="Z11" s="1"/>
+      <c r="AE11" s="1"/>
+      <c r="AI11" s="1"/>
+      <c r="AK11" s="1"/>
+    </row>
+    <row r="12" spans="1:40" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="9"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+      <c r="K12" s="1"/>
+      <c r="L12" s="1"/>
+      <c r="X12" s="1"/>
+      <c r="Z12" s="1"/>
+      <c r="AE12" s="1"/>
+      <c r="AI12" s="1"/>
+      <c r="AK12" s="1"/>
+    </row>
+    <row r="13" spans="1:40" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="L13" s="1"/>
+      <c r="Q13" s="1"/>
+      <c r="R13" s="1"/>
+      <c r="S13" s="1"/>
+      <c r="X13" s="1"/>
+      <c r="Z13" s="1"/>
+      <c r="AE13" s="1"/>
+      <c r="AF13" s="1"/>
+      <c r="AG13" s="1"/>
+      <c r="AH13" s="1"/>
+      <c r="AI13" s="1"/>
+      <c r="AK13" s="1"/>
+      <c r="AL13" s="1"/>
+      <c r="AM13" s="1"/>
+    </row>
+    <row r="14" spans="1:40" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="L14" s="1"/>
+      <c r="Q14" s="1"/>
+      <c r="S14" s="1"/>
+      <c r="X14" s="1"/>
+      <c r="Z14" s="1"/>
+      <c r="AM14" s="1"/>
+    </row>
+    <row r="15" spans="1:40" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="9"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="1"/>
+      <c r="K15" s="1"/>
+      <c r="L15" s="1"/>
+      <c r="Q15" s="1"/>
+      <c r="S15" s="1"/>
+      <c r="X15" s="1"/>
+      <c r="Z15" s="1"/>
+      <c r="AH15" s="1"/>
+      <c r="AM15" s="1"/>
+    </row>
+    <row r="16" spans="1:40" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="Q16" s="1"/>
+      <c r="S16" s="1"/>
+      <c r="X16" s="1"/>
+      <c r="Y16" s="1"/>
+      <c r="Z16" s="1"/>
+      <c r="AM16" s="1"/>
+    </row>
+    <row r="17" spans="1:39" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E17" s="1"/>
+      <c r="Q17" s="1"/>
+      <c r="S17" s="1"/>
+      <c r="AI17" s="1"/>
+      <c r="AM17" s="1"/>
+    </row>
+    <row r="18" spans="1:39" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="N18" s="1"/>
+      <c r="Q18" s="1"/>
+      <c r="S18" s="1"/>
+      <c r="AF18" s="1"/>
+      <c r="AG18" s="1"/>
+      <c r="AH18" s="1"/>
+      <c r="AI18" s="1"/>
+      <c r="AJ18" s="1"/>
+      <c r="AK18" s="1"/>
+      <c r="AL18" s="1"/>
+      <c r="AM18" s="1"/>
+    </row>
+    <row r="19" spans="1:39" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="Q19" s="1"/>
+      <c r="S19" s="1"/>
+      <c r="Y19" s="1"/>
+      <c r="AF19" s="1"/>
+    </row>
+    <row r="20" spans="1:39" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="9"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1"/>
+      <c r="I20" s="1"/>
+      <c r="J20" s="1"/>
+      <c r="K20" s="1"/>
+      <c r="L20" s="1"/>
+      <c r="M20" s="1"/>
+      <c r="N20" s="1"/>
+      <c r="O20" s="1"/>
+      <c r="P20" s="1"/>
+      <c r="Q20" s="1"/>
+      <c r="S20" s="1"/>
+      <c r="AF20" s="1"/>
+    </row>
+    <row r="21" spans="1:39" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="S21" s="1"/>
+      <c r="T21" s="1"/>
+      <c r="U21" s="1"/>
+      <c r="V21" s="1"/>
+      <c r="W21" s="1"/>
+      <c r="X21" s="1"/>
+      <c r="Y21" s="1"/>
+      <c r="Z21" s="1"/>
+      <c r="AA21" s="1"/>
+      <c r="AB21" s="1"/>
+      <c r="AC21" s="1"/>
+      <c r="AD21" s="1"/>
+      <c r="AE21" s="1"/>
+      <c r="AF21" s="1"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
change the confiures in level1, 2, 3, 4
</commit_message>
<xml_diff>
--- a/docs/config/levels.xlsx
+++ b/docs/config/levels.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\yyy\software_engine\2025-group-5\docs\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{571E3501-F3F2-48F1-BFEE-68ED288654D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0538DCB2-7A83-4A24-8C65-B06D9D033CDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="3" xr2:uid="{9F8622C9-03A3-4207-9844-CBC14631E7E3}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{9F8622C9-03A3-4207-9844-CBC14631E7E3}"/>
   </bookViews>
   <sheets>
     <sheet name="level1" sheetId="1" r:id="rId1"/>
@@ -34,10 +34,6 @@
     </ext>
   </extLst>
 </workbook>
-</file>
-
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -494,9 +490,9 @@
       <selection activeCell="AM14" sqref="AM14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="3.58203125" defaultRowHeight="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="3.625" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="4" spans="1:40" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:40" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="T4" s="1"/>
       <c r="U4" s="1"/>
       <c r="V4" s="1"/>
@@ -517,7 +513,7 @@
       <c r="AM4" s="2"/>
       <c r="AN4" s="2"/>
     </row>
-    <row r="5" spans="1:40" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:40" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="N5" s="1"/>
       <c r="O5" s="1"/>
       <c r="P5" s="1"/>
@@ -536,7 +532,7 @@
       <c r="AM5" s="1"/>
       <c r="AN5" s="1"/>
     </row>
-    <row r="6" spans="1:40" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:40" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="N6" s="1"/>
       <c r="Z6" s="1"/>
       <c r="AA6" s="1"/>
@@ -545,7 +541,7 @@
       <c r="AH6" s="1"/>
       <c r="AN6" s="1"/>
     </row>
-    <row r="7" spans="1:40" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:40" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="N7" s="2"/>
       <c r="Z7" s="1"/>
       <c r="AA7" s="1"/>
@@ -557,7 +553,7 @@
       <c r="AK7" s="1"/>
       <c r="AN7" s="1"/>
     </row>
-    <row r="8" spans="1:40" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:40" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="N8" s="2"/>
       <c r="T8" s="1"/>
       <c r="U8" s="1"/>
@@ -567,7 +563,7 @@
       <c r="AL8" s="1"/>
       <c r="AN8" s="1"/>
     </row>
-    <row r="9" spans="1:40" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:40" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="N9" s="2"/>
       <c r="T9" s="1"/>
       <c r="U9" s="1"/>
@@ -576,7 +572,7 @@
       <c r="Z9" s="1"/>
       <c r="AN9" s="1"/>
     </row>
-    <row r="10" spans="1:40" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:40" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="N10" s="2"/>
       <c r="P10" s="1"/>
       <c r="Q10" s="1"/>
@@ -587,14 +583,14 @@
       <c r="Z10" s="1"/>
       <c r="AN10" s="1"/>
     </row>
-    <row r="11" spans="1:40" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:40" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="N11" s="2"/>
       <c r="P11" s="1"/>
       <c r="Q11" s="1"/>
       <c r="Z11" s="1"/>
       <c r="AN11" s="1"/>
     </row>
-    <row r="12" spans="1:40" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:40" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
@@ -611,7 +607,7 @@
       <c r="AA12" s="1"/>
       <c r="AN12" s="1"/>
     </row>
-    <row r="13" spans="1:40" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:40" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -625,7 +621,7 @@
       <c r="AH13" s="1"/>
       <c r="AN13" s="1"/>
     </row>
-    <row r="14" spans="1:40" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:40" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="P14" s="1"/>
       <c r="Q14" s="1"/>
       <c r="S14" s="1"/>
@@ -634,7 +630,7 @@
       <c r="AH14" s="1"/>
       <c r="AN14" s="1"/>
     </row>
-    <row r="15" spans="1:40" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:40" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="P15" s="1"/>
       <c r="Q15" s="1"/>
       <c r="S15" s="1"/>
@@ -643,7 +639,7 @@
       <c r="AH15" s="1"/>
       <c r="AN15" s="1"/>
     </row>
-    <row r="16" spans="1:40" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:40" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="1"/>
       <c r="G16" s="1"/>
       <c r="I16" s="1"/>
@@ -656,7 +652,7 @@
       <c r="AH16" s="1"/>
       <c r="AN16" s="1"/>
     </row>
-    <row r="17" spans="1:40" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:40" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="1"/>
       <c r="G17" s="1"/>
       <c r="P17" s="1"/>
@@ -665,7 +661,7 @@
       <c r="AA17" s="1"/>
       <c r="AN17" s="1"/>
     </row>
-    <row r="18" spans="1:40" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:40" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="1"/>
       <c r="G18" s="1"/>
       <c r="J18" s="1"/>
@@ -674,7 +670,7 @@
       <c r="Z18" s="1"/>
       <c r="AN18" s="1"/>
     </row>
-    <row r="19" spans="1:40" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:40" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="1"/>
       <c r="P19" s="1"/>
       <c r="Q19" s="1"/>
@@ -685,7 +681,7 @@
       <c r="Z19" s="1"/>
       <c r="AN19" s="1"/>
     </row>
-    <row r="20" spans="1:40" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:40" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="T20" s="1"/>
@@ -695,7 +691,7 @@
       <c r="Z20" s="1"/>
       <c r="AN20" s="1"/>
     </row>
-    <row r="21" spans="1:40" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:40" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
       <c r="G21" s="1"/>
@@ -710,7 +706,7 @@
       <c r="AC21" s="1"/>
       <c r="AN21" s="1"/>
     </row>
-    <row r="22" spans="1:40" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:40" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C22" s="1"/>
       <c r="G22" s="1"/>
       <c r="K22" s="1"/>
@@ -726,7 +722,7 @@
       <c r="AM22" s="1"/>
       <c r="AN22" s="1"/>
     </row>
-    <row r="23" spans="1:40" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:40" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
       <c r="G23" s="1"/>
@@ -740,7 +736,7 @@
       <c r="AJ23" s="1"/>
       <c r="AN23" s="1"/>
     </row>
-    <row r="24" spans="1:40" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:40" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D24" s="1"/>
       <c r="G24" s="1"/>
       <c r="H24" s="1"/>
@@ -757,7 +753,7 @@
       <c r="AJ24" s="1"/>
       <c r="AN24" s="1"/>
     </row>
-    <row r="25" spans="1:40" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:40" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D25" s="1"/>
       <c r="G25" s="1"/>
       <c r="O25" s="1"/>
@@ -796,9 +792,9 @@
       <selection activeCell="AR7" sqref="AR7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="3.58203125" defaultRowHeight="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="3.625" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:40" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:40" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -819,7 +815,7 @@
       <c r="V1" s="1"/>
       <c r="AN1" s="1"/>
     </row>
-    <row r="2" spans="1:40" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:40" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -834,7 +830,7 @@
       <c r="V2" s="1"/>
       <c r="AN2" s="1"/>
     </row>
-    <row r="3" spans="1:40" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:40" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -850,7 +846,7 @@
       <c r="V3" s="1"/>
       <c r="AN3" s="1"/>
     </row>
-    <row r="4" spans="1:40" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:40" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -865,7 +861,7 @@
       <c r="V4" s="1"/>
       <c r="AN4" s="1"/>
     </row>
-    <row r="5" spans="1:40" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:40" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -878,7 +874,7 @@
       <c r="V5" s="1"/>
       <c r="AN5" s="1"/>
     </row>
-    <row r="6" spans="1:40" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:40" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -891,7 +887,7 @@
       <c r="V6" s="1"/>
       <c r="AN6" s="1"/>
     </row>
-    <row r="7" spans="1:40" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:40" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -904,7 +900,7 @@
       <c r="V7" s="1"/>
       <c r="AN7" s="1"/>
     </row>
-    <row r="8" spans="1:40" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:40" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -920,7 +916,7 @@
       <c r="AG8" s="1"/>
       <c r="AN8" s="1"/>
     </row>
-    <row r="9" spans="1:40" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:40" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -940,7 +936,7 @@
       <c r="AG9" s="1"/>
       <c r="AN9" s="1"/>
     </row>
-    <row r="10" spans="1:40" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:40" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -960,7 +956,7 @@
       <c r="AJ10" s="1"/>
       <c r="AN10" s="1"/>
     </row>
-    <row r="11" spans="1:40" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:40" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -989,7 +985,7 @@
       <c r="AM11" s="1"/>
       <c r="AN11" s="1"/>
     </row>
-    <row r="12" spans="1:40" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:40" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -1020,7 +1016,7 @@
       <c r="AK12" s="1"/>
       <c r="AN12" s="1"/>
     </row>
-    <row r="13" spans="1:40" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:40" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -1039,20 +1035,20 @@
       <c r="AH13" s="1"/>
       <c r="AN13" s="1"/>
     </row>
-    <row r="14" spans="1:40" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:40" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
     </row>
-    <row r="15" spans="1:40" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:40" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
       <c r="AG15" s="1"/>
     </row>
-    <row r="16" spans="1:40" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:40" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -1071,7 +1067,7 @@
       <c r="AM16" s="1"/>
       <c r="AN16" s="1"/>
     </row>
-    <row r="17" spans="1:40" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:40" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -1100,7 +1096,7 @@
       <c r="AM17" s="1"/>
       <c r="AN17" s="1"/>
     </row>
-    <row r="18" spans="1:40" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:40" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -1134,7 +1130,7 @@
       <c r="AM18" s="1"/>
       <c r="AN18" s="1"/>
     </row>
-    <row r="19" spans="1:40" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:40" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -1162,7 +1158,7 @@
       <c r="AM19" s="1"/>
       <c r="AN19" s="1"/>
     </row>
-    <row r="20" spans="1:40" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:40" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -1188,7 +1184,7 @@
       <c r="AM20" s="1"/>
       <c r="AN20" s="1"/>
     </row>
-    <row r="21" spans="1:40" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:40" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -1204,7 +1200,7 @@
       <c r="AM21" s="1"/>
       <c r="AN21" s="1"/>
     </row>
-    <row r="22" spans="1:40" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:40" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="1"/>
       <c r="M22" s="1"/>
       <c r="N22" s="1"/>
@@ -1228,7 +1224,7 @@
       <c r="AM22" s="1"/>
       <c r="AN22" s="1"/>
     </row>
-    <row r="23" spans="1:40" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:40" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="1"/>
       <c r="D23" s="1"/>
       <c r="M23" s="1"/>
@@ -1253,7 +1249,7 @@
       <c r="AM23" s="1"/>
       <c r="AN23" s="1"/>
     </row>
-    <row r="24" spans="1:40" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:40" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="1"/>
       <c r="M24" s="1"/>
       <c r="N24" s="1"/>
@@ -1271,7 +1267,7 @@
       <c r="AM24" s="1"/>
       <c r="AN24" s="1"/>
     </row>
-    <row r="25" spans="1:40" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:40" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -1310,12 +1306,12 @@
   <dimension ref="A1:AO27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+      <selection activeCell="AE13" sqref="AE13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="3.58203125" defaultRowHeight="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="3.625" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:41" ht="20.149999999999999" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:41" ht="20.100000000000001" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="F1" s="3"/>
       <c r="G1" s="4"/>
       <c r="H1" s="3"/>
@@ -1323,20 +1319,22 @@
       <c r="AA1" s="4"/>
       <c r="AB1" s="4"/>
       <c r="AC1" s="4"/>
-      <c r="AD1" s="4"/>
-      <c r="AE1" s="4"/>
+      <c r="AD1" s="3"/>
+      <c r="AE1" s="3"/>
       <c r="AF1" s="4"/>
       <c r="AG1" s="4"/>
       <c r="AH1" s="4"/>
       <c r="AI1" s="3"/>
     </row>
-    <row r="2" spans="1:41" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:41" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F2" s="1"/>
       <c r="H2" s="1"/>
       <c r="Z2" s="1"/>
+      <c r="AD2" s="1"/>
+      <c r="AE2" s="1"/>
       <c r="AI2" s="1"/>
     </row>
-    <row r="3" spans="1:41" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:41" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
@@ -1347,13 +1345,18 @@
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
       <c r="Y3" s="1"/>
+      <c r="AD3" s="1"/>
       <c r="AI3" s="1"/>
     </row>
-    <row r="4" spans="1:41" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:41" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" s="1"/>
       <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1"/>
+      <c r="M4" s="1"/>
       <c r="N4" s="1"/>
       <c r="O4" s="1"/>
       <c r="P4" s="1"/>
@@ -1381,12 +1384,19 @@
       <c r="AM4" s="6"/>
       <c r="AN4" s="7"/>
     </row>
-    <row r="5" spans="1:41" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:41" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
-    </row>
-    <row r="6" spans="1:41" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
+    </row>
+    <row r="6" spans="1:41" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D6" s="1"/>
+      <c r="K6" s="1"/>
+      <c r="O6" s="1"/>
       <c r="P6" s="1"/>
       <c r="Q6" s="1"/>
       <c r="R6" s="1"/>
@@ -1405,7 +1415,7 @@
       <c r="AM6" s="1"/>
       <c r="AN6" s="8"/>
     </row>
-    <row r="7" spans="1:41" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:41" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D7" s="1"/>
       <c r="N7" s="6"/>
       <c r="O7" s="1"/>
@@ -1419,7 +1429,7 @@
       <c r="AI7" s="1"/>
       <c r="AJ7" s="1"/>
     </row>
-    <row r="8" spans="1:41" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:41" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="9"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -1429,7 +1439,7 @@
       <c r="AF8" s="1"/>
       <c r="AK8" s="1"/>
     </row>
-    <row r="9" spans="1:41" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:41" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="10"/>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
@@ -1448,7 +1458,7 @@
       <c r="AJ9" s="1"/>
       <c r="AK9" s="1"/>
     </row>
-    <row r="10" spans="1:41" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:41" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="9"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -1459,7 +1469,7 @@
       <c r="X10" s="1"/>
       <c r="AH10" s="1"/>
     </row>
-    <row r="11" spans="1:41" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:41" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B11" s="1"/>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
@@ -1471,7 +1481,7 @@
       <c r="Z11" s="1"/>
       <c r="AH11" s="1"/>
     </row>
-    <row r="12" spans="1:41" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:41" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="1"/>
       <c r="K12" s="1"/>
       <c r="O12" s="1"/>
@@ -1482,7 +1492,7 @@
       <c r="AG12" s="1"/>
       <c r="AH12" s="1"/>
     </row>
-    <row r="13" spans="1:41" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:41" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
@@ -1496,7 +1506,7 @@
       <c r="AE13" s="1"/>
       <c r="AF13" s="1"/>
     </row>
-    <row r="14" spans="1:41" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:41" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14" s="1"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
@@ -1506,7 +1516,7 @@
       <c r="AA14" s="1"/>
       <c r="AC14" s="1"/>
     </row>
-    <row r="15" spans="1:41" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:41" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B15" s="1"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
@@ -1521,7 +1531,7 @@
       <c r="AC15" s="1"/>
       <c r="AN15" s="8"/>
     </row>
-    <row r="16" spans="1:41" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:41" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B16" s="1"/>
       <c r="D16" s="1"/>
       <c r="M16" s="1"/>
@@ -1529,10 +1539,10 @@
       <c r="AA16" s="1"/>
       <c r="AC16" s="1"/>
       <c r="AM16" s="1"/>
-      <c r="AN16" s="5"/>
+      <c r="AN16" s="6"/>
       <c r="AO16" s="5"/>
     </row>
-    <row r="17" spans="1:41" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:41" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B17" s="1"/>
       <c r="D17" s="1"/>
       <c r="M17" s="1"/>
@@ -1547,16 +1557,19 @@
       <c r="AA17" s="1"/>
       <c r="AC17" s="1"/>
       <c r="AL17" s="1"/>
-      <c r="AN17" s="5"/>
+      <c r="AM17" s="1"/>
+      <c r="AN17" s="6"/>
       <c r="AO17" s="5"/>
     </row>
-    <row r="18" spans="1:41" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:41" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="9"/>
       <c r="B18" s="1"/>
       <c r="D18" s="1"/>
       <c r="M18" s="1"/>
       <c r="O18" s="1"/>
       <c r="S18" s="1"/>
+      <c r="X18" s="1"/>
+      <c r="Y18" s="1"/>
       <c r="Z18" s="1"/>
       <c r="AA18" s="1"/>
       <c r="AC18" s="1"/>
@@ -1564,20 +1577,23 @@
       <c r="AN18" s="5"/>
       <c r="AO18" s="5"/>
     </row>
-    <row r="19" spans="1:41" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:41" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B19" s="1"/>
       <c r="D19" s="1"/>
       <c r="M19" s="1"/>
       <c r="P19" s="1"/>
       <c r="Q19" s="1"/>
       <c r="R19" s="1"/>
+      <c r="X19" s="1"/>
+      <c r="Y19" s="1"/>
       <c r="AC19" s="1"/>
       <c r="AD19" s="1"/>
       <c r="AJ19" s="1"/>
-      <c r="AN19" s="5"/>
+      <c r="AM19" s="1"/>
+      <c r="AN19" s="6"/>
       <c r="AO19" s="5"/>
     </row>
-    <row r="20" spans="1:41" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:41" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
       <c r="M20" s="1"/>
@@ -1586,7 +1602,7 @@
       <c r="AN20" s="5"/>
       <c r="AO20" s="5"/>
     </row>
-    <row r="21" spans="1:41" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:41" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
       <c r="M21" s="1"/>
@@ -1600,7 +1616,7 @@
       <c r="AN21" s="5"/>
       <c r="AO21" s="5"/>
     </row>
-    <row r="22" spans="1:41" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:41" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
@@ -1623,14 +1639,14 @@
       <c r="AN22" s="5"/>
       <c r="AO22" s="5"/>
     </row>
-    <row r="23" spans="1:41" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:41" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="U23" s="1"/>
       <c r="V23" s="1"/>
       <c r="W23" s="1"/>
       <c r="AN23" s="5"/>
       <c r="AO23" s="5"/>
     </row>
-    <row r="24" spans="1:41" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:41" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
       <c r="J24" s="1"/>
@@ -1639,6 +1655,8 @@
       <c r="M24" s="1"/>
       <c r="N24" s="1"/>
       <c r="O24" s="1"/>
+      <c r="V24" s="1"/>
+      <c r="W24" s="1"/>
       <c r="AE24" s="1"/>
       <c r="AF24" s="1"/>
       <c r="AG24" s="1"/>
@@ -1647,9 +1665,10 @@
       <c r="AN24" s="5"/>
       <c r="AO24" s="5"/>
     </row>
-    <row r="25" spans="1:41" ht="20.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:41" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="I25" s="11"/>
       <c r="P25" s="11"/>
+      <c r="V25" s="1"/>
       <c r="Z25" s="11"/>
       <c r="AA25" s="11"/>
       <c r="AB25" s="11"/>
@@ -1658,15 +1677,15 @@
       <c r="AE25" s="11"/>
       <c r="AG25" s="11"/>
       <c r="AH25" s="5"/>
-      <c r="AI25" s="5"/>
-      <c r="AJ25" s="5"/>
+      <c r="AI25" s="6"/>
+      <c r="AJ25" s="6"/>
       <c r="AK25" s="5"/>
       <c r="AL25" s="5"/>
       <c r="AM25" s="5"/>
       <c r="AN25" s="5"/>
       <c r="AO25" s="5"/>
     </row>
-    <row r="26" spans="1:41" ht="20.149999999999999" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:41" ht="20.100000000000001" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="AH26" s="5"/>
       <c r="AI26" s="5"/>
       <c r="AJ26" s="5"/>
@@ -1675,7 +1694,7 @@
       <c r="AM26" s="5"/>
       <c r="AN26" s="5"/>
     </row>
-    <row r="27" spans="1:41" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:41" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AH27" s="5"/>
       <c r="AI27" s="5"/>
       <c r="AJ27" s="5"/>
@@ -1694,13 +1713,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B873F3A3-FC30-4AC8-9328-E2AAE444BD5F}">
   <dimension ref="A2:AN21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="S30" sqref="S30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H19" sqref="H19:I19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="3.58203125" defaultRowHeight="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="3.625" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="2" spans="1:40" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:40" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>
@@ -1712,12 +1731,12 @@
       <c r="S2" s="1"/>
       <c r="T2" s="1"/>
     </row>
-    <row r="3" spans="1:40" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:40" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
       <c r="T3" s="1"/>
     </row>
-    <row r="4" spans="1:40" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:40" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="I4" s="1"/>
       <c r="T4" s="1"/>
       <c r="Z4" s="1"/>
@@ -1736,7 +1755,7 @@
       <c r="AM4" s="6"/>
       <c r="AN4" s="7"/>
     </row>
-    <row r="5" spans="1:40" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:40" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="I5" s="1"/>
       <c r="T5" s="1"/>
       <c r="U5" s="1"/>
@@ -1746,10 +1765,10 @@
       <c r="Y5" s="1"/>
       <c r="Z5" s="1"/>
     </row>
-    <row r="6" spans="1:40" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:40" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="I6" s="1"/>
     </row>
-    <row r="7" spans="1:40" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:40" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="I7" s="1"/>
       <c r="T7" s="1"/>
       <c r="U7" s="1"/>
@@ -1760,7 +1779,7 @@
       <c r="Z7" s="1"/>
       <c r="AK7" s="1"/>
     </row>
-    <row r="8" spans="1:40" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:40" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="9"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -1773,11 +1792,15 @@
       <c r="N8" s="5"/>
       <c r="T8" s="1"/>
       <c r="Z8" s="1"/>
-    </row>
-    <row r="9" spans="1:40" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AH8" s="1"/>
+      <c r="AI8" s="1"/>
+    </row>
+    <row r="9" spans="1:40" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="J9" s="1"/>
       <c r="N9" s="5"/>
       <c r="O9" s="1"/>
+      <c r="R9" s="1"/>
+      <c r="S9" s="1"/>
       <c r="T9" s="1"/>
       <c r="Z9" s="1"/>
       <c r="AE9" s="1"/>
@@ -1790,8 +1813,10 @@
       <c r="AM9" s="1"/>
       <c r="AN9" s="8"/>
     </row>
-    <row r="10" spans="1:40" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:40" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="N10" s="5"/>
+      <c r="R10" s="1"/>
+      <c r="S10" s="1"/>
       <c r="T10" s="1"/>
       <c r="U10" s="1"/>
       <c r="V10" s="1"/>
@@ -1802,7 +1827,7 @@
       <c r="AI10" s="1"/>
       <c r="AK10" s="1"/>
     </row>
-    <row r="11" spans="1:40" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:40" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="N11" s="5"/>
       <c r="X11" s="1"/>
       <c r="Z11" s="1"/>
@@ -1810,7 +1835,7 @@
       <c r="AI11" s="1"/>
       <c r="AK11" s="1"/>
     </row>
-    <row r="12" spans="1:40" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:40" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="9"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -1829,7 +1854,7 @@
       <c r="AI12" s="1"/>
       <c r="AK12" s="1"/>
     </row>
-    <row r="13" spans="1:40" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:40" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="L13" s="1"/>
       <c r="Q13" s="1"/>
       <c r="R13" s="1"/>
@@ -1845,7 +1870,7 @@
       <c r="AL13" s="1"/>
       <c r="AM13" s="1"/>
     </row>
-    <row r="14" spans="1:40" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:40" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="L14" s="1"/>
       <c r="Q14" s="1"/>
       <c r="S14" s="1"/>
@@ -1853,7 +1878,7 @@
       <c r="Z14" s="1"/>
       <c r="AM14" s="1"/>
     </row>
-    <row r="15" spans="1:40" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:40" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="9"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -1873,7 +1898,7 @@
       <c r="AH15" s="1"/>
       <c r="AM15" s="1"/>
     </row>
-    <row r="16" spans="1:40" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:40" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="Q16" s="1"/>
       <c r="S16" s="1"/>
       <c r="X16" s="1"/>
@@ -1881,14 +1906,14 @@
       <c r="Z16" s="1"/>
       <c r="AM16" s="1"/>
     </row>
-    <row r="17" spans="1:39" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:39" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E17" s="1"/>
       <c r="Q17" s="1"/>
       <c r="S17" s="1"/>
       <c r="AI17" s="1"/>
       <c r="AM17" s="1"/>
     </row>
-    <row r="18" spans="1:39" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:39" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="N18" s="1"/>
       <c r="Q18" s="1"/>
       <c r="S18" s="1"/>
@@ -1901,13 +1926,15 @@
       <c r="AL18" s="1"/>
       <c r="AM18" s="1"/>
     </row>
-    <row r="19" spans="1:39" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:39" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
       <c r="Q19" s="1"/>
       <c r="S19" s="1"/>
       <c r="Y19" s="1"/>
       <c r="AF19" s="1"/>
     </row>
-    <row r="20" spans="1:39" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:39" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="9"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -1928,7 +1955,7 @@
       <c r="S20" s="1"/>
       <c r="AF20" s="1"/>
     </row>
-    <row r="21" spans="1:39" ht="20.149999999999999" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:39" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="S21" s="1"/>
       <c r="T21" s="1"/>
       <c r="U21" s="1"/>

</xml_diff>